<commit_message>
Added stats for telecommunication
</commit_message>
<xml_diff>
--- a/ZippiaTop100Data/Zippia Initial Stats Analysis.xlsx
+++ b/ZippiaTop100Data/Zippia Initial Stats Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fucky\Documents\ZippiaTop100Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBE27C9C-CC22-4163-BE6F-F79AFC7CE4BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DAAD0EB-F137-4C92-BC27-E93B2612E571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F9D06C72-0A29-4EF6-AB7B-2E80CBBF3E7F}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{F9D06C72-0A29-4EF6-AB7B-2E80CBBF3E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="17">
   <si>
     <t>Employees Who Are Women</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Transportation</t>
+  </si>
+  <si>
+    <t>Telecommunication</t>
   </si>
 </sst>
 </file>
@@ -670,16 +673,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B570C8D4-3A1E-4F6D-9663-005C8CFA258D}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3:D5"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42:A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="24.6640625" customWidth="1"/>
     <col min="4" max="4" width="24.88671875" customWidth="1"/>
@@ -1195,8 +1198,59 @@
         <v>0.32</v>
       </c>
     </row>
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="17">
+        <v>90</v>
+      </c>
+      <c r="D42" s="18">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="24"/>
+      <c r="B43" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="15">
+        <v>0.36155555555555563</v>
+      </c>
+      <c r="D43" s="19">
+        <v>0.31907894736842091</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="24"/>
+      <c r="B44" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" s="15">
+        <v>0.36</v>
+      </c>
+      <c r="D44" s="19">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="25"/>
+      <c r="B45" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" s="21">
+        <v>0.36</v>
+      </c>
+      <c r="D45" s="22">
+        <v>0.33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A42:A45"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A38:A41"/>
     <mergeCell ref="A34:A37"/>

</xml_diff>